<commit_message>
New dataset test complete
</commit_message>
<xml_diff>
--- a/verification.xlsx
+++ b/verification.xlsx
@@ -19,13 +19,13 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="72" uniqueCount="48">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="81" uniqueCount="48">
   <si>
     <t>FSS手法によるフィーチャエンジニアリング</t>
     <rPh sb="3" eb="5">
       <t>シュホウ</t>
     </rPh>
-    <phoneticPr fontId="2"/>
+    <phoneticPr fontId="3"/>
   </si>
   <si>
     <t>特徴量</t>
@@ -35,177 +35,173 @@
     <rPh sb="2" eb="3">
       <t>リョウ</t>
     </rPh>
-    <phoneticPr fontId="2"/>
+    <phoneticPr fontId="3"/>
   </si>
   <si>
     <t>PITCH</t>
-    <phoneticPr fontId="2"/>
+    <phoneticPr fontId="3"/>
   </si>
   <si>
     <t>訓練acc</t>
     <rPh sb="0" eb="2">
       <t>クンレン</t>
     </rPh>
-    <phoneticPr fontId="2"/>
+    <phoneticPr fontId="3"/>
   </si>
   <si>
     <t>訓練loss</t>
     <rPh sb="0" eb="2">
       <t>クンレン</t>
     </rPh>
-    <phoneticPr fontId="2"/>
+    <phoneticPr fontId="3"/>
   </si>
   <si>
     <t>検証acc</t>
     <rPh sb="0" eb="2">
       <t>ケンショウ</t>
     </rPh>
-    <phoneticPr fontId="2"/>
+    <phoneticPr fontId="3"/>
   </si>
   <si>
     <t>検証loss</t>
     <rPh sb="0" eb="2">
       <t>ケンショウ</t>
     </rPh>
-    <phoneticPr fontId="2"/>
+    <phoneticPr fontId="3"/>
   </si>
   <si>
     <t>テストacc</t>
-    <phoneticPr fontId="2"/>
+    <phoneticPr fontId="3"/>
   </si>
   <si>
     <t>テストloss</t>
-    <phoneticPr fontId="2"/>
+    <phoneticPr fontId="3"/>
   </si>
   <si>
     <t>VOLUME</t>
-    <phoneticPr fontId="2"/>
+    <phoneticPr fontId="3"/>
   </si>
   <si>
     <t>TEMPO</t>
-    <phoneticPr fontId="2"/>
+    <phoneticPr fontId="3"/>
   </si>
   <si>
     <t>MFCC + PITCH</t>
-    <phoneticPr fontId="2"/>
+    <phoneticPr fontId="3"/>
   </si>
   <si>
     <t>MFCC + VOLUME</t>
-    <phoneticPr fontId="2"/>
+    <phoneticPr fontId="3"/>
   </si>
   <si>
     <t>MFCC + TEMPO</t>
-    <phoneticPr fontId="2"/>
+    <phoneticPr fontId="3"/>
   </si>
   <si>
     <t>MFCC</t>
-    <phoneticPr fontId="2"/>
+    <phoneticPr fontId="3"/>
   </si>
   <si>
     <t>CNN_RNN_BiLSTM_2020-02-19_final05_86.2%_model.h5</t>
-    <phoneticPr fontId="2"/>
-  </si>
-  <si>
-    <t>model name</t>
-    <phoneticPr fontId="2"/>
+    <phoneticPr fontId="3"/>
   </si>
   <si>
     <t>CNN_RNN_BiLSTM_2020-02-19_final05_15.5%_model.h5</t>
-    <phoneticPr fontId="2"/>
+    <phoneticPr fontId="3"/>
   </si>
   <si>
     <t>CNN_RNN_BiLSTM_2020-02-19_final06_69.0%_model.h5</t>
-    <phoneticPr fontId="2"/>
+    <phoneticPr fontId="3"/>
   </si>
   <si>
     <t>CNN_RNN_BiLSTM_2020-02-20_final03_15.5%_model.h5</t>
-    <phoneticPr fontId="2"/>
+    <phoneticPr fontId="3"/>
   </si>
   <si>
     <t>CNN_RNN_BiLSTM_2020-02-23_final03_87.3%_model.h5</t>
-    <phoneticPr fontId="2"/>
+    <phoneticPr fontId="3"/>
   </si>
   <si>
     <t>CNN_RNN_BiLSTM_2020-02-25_final02_88.1%_model.h5</t>
-    <phoneticPr fontId="2"/>
+    <phoneticPr fontId="3"/>
   </si>
   <si>
     <t>CNN_RNN_BiLSTM_2020-02-26_final02_85.3%_model.h5</t>
-    <phoneticPr fontId="2"/>
+    <phoneticPr fontId="3"/>
   </si>
   <si>
     <t>MFCC + TEMPO + PITCH</t>
-    <phoneticPr fontId="2"/>
+    <phoneticPr fontId="3"/>
   </si>
   <si>
     <t>MFCC +TEMPO + VOLUME</t>
-    <phoneticPr fontId="2"/>
+    <phoneticPr fontId="3"/>
   </si>
   <si>
     <t>CNN_RNN_BiLSTM_2020-02-27_final08_85.6%_model.h5</t>
-    <phoneticPr fontId="2"/>
+    <phoneticPr fontId="3"/>
   </si>
   <si>
     <t>CNN_RNN_BiLSTM_2020-02-27_final10_88.0%_model.h5</t>
-    <phoneticPr fontId="2"/>
+    <phoneticPr fontId="3"/>
   </si>
   <si>
     <t>MFCC + TEMPO + VOLUME + PITCH</t>
-    <phoneticPr fontId="2"/>
+    <phoneticPr fontId="3"/>
   </si>
   <si>
     <t>CNN_RNN_BiLSTM_2020-02-29_final07_88.6%_model.h5</t>
-    <phoneticPr fontId="2"/>
+    <phoneticPr fontId="3"/>
   </si>
   <si>
     <t>Data set No.1（外たれOnly）&amp; Data Augument &amp;  500epoch</t>
     <rPh sb="14" eb="15">
       <t>ガイ</t>
     </rPh>
-    <phoneticPr fontId="2"/>
+    <phoneticPr fontId="3"/>
   </si>
   <si>
     <t>Data set No.2（日本人Only）&amp; Data Augument &amp; 500epoch</t>
     <rPh sb="14" eb="17">
       <t>ニホンジン</t>
     </rPh>
-    <phoneticPr fontId="2"/>
+    <phoneticPr fontId="3"/>
   </si>
   <si>
     <t>CNN_RNN_BiLSTM_2020-03-01_final01_99.6%_model.h5</t>
-    <phoneticPr fontId="2"/>
+    <phoneticPr fontId="3"/>
   </si>
   <si>
     <t>CNN_RNN_BiLSTM_2020-03-01_final04_92.5%_model.h5</t>
-    <phoneticPr fontId="2"/>
+    <phoneticPr fontId="3"/>
   </si>
   <si>
     <t>CNN_RNN_BiLSTM_2020-03-02_final02_93.7%_model.h5</t>
-    <phoneticPr fontId="2"/>
+    <phoneticPr fontId="3"/>
   </si>
   <si>
     <t>CNN_RNN_BiLSTM_2020-03-06_final03_33.4%_model.h5</t>
-    <phoneticPr fontId="2"/>
+    <phoneticPr fontId="3"/>
   </si>
   <si>
     <t>CNN_RNN_BiLSTM_2020-03-07_final09_99.8%_model.h5</t>
-    <phoneticPr fontId="2"/>
+    <phoneticPr fontId="3"/>
   </si>
   <si>
     <t>CNN_RNN_BiLSTM_2020-03-07_final10_99.9%_model.h5</t>
-    <phoneticPr fontId="2"/>
+    <phoneticPr fontId="3"/>
   </si>
   <si>
     <t>CNN_RNN_BiLSTM_2020-03-08_final06_99.7%_model.h5</t>
-    <phoneticPr fontId="2"/>
+    <phoneticPr fontId="3"/>
   </si>
   <si>
     <t>MFCC + PITCH + TEMPO</t>
-    <phoneticPr fontId="2"/>
+    <phoneticPr fontId="3"/>
   </si>
   <si>
     <t>MFCC + PITCH + VOLUME</t>
-    <phoneticPr fontId="2"/>
+    <phoneticPr fontId="3"/>
   </si>
   <si>
     <r>
@@ -232,15 +228,15 @@
       </rPr>
       <t>OLUME</t>
     </r>
-    <phoneticPr fontId="2"/>
+    <phoneticPr fontId="3"/>
   </si>
   <si>
     <t>CNN_RNN_BiLSTM_2020-03-08_final03_99.6%_model.h5</t>
-    <phoneticPr fontId="2"/>
+    <phoneticPr fontId="3"/>
   </si>
   <si>
     <t>CNN_RNN_BiLSTM_2020-03-09_final06_99.8%_model.h5</t>
-    <phoneticPr fontId="2"/>
+    <phoneticPr fontId="3"/>
   </si>
   <si>
     <t>CNN_RNN_BiLSTM_2022-02-17_final03_80.3%_model.h5</t>
@@ -253,30 +249,54 @@
     <rPh sb="19" eb="21">
       <t>ガイジン</t>
     </rPh>
-    <phoneticPr fontId="2"/>
-  </si>
-  <si>
-    <t>process_model_06_2022-02-19-00-07-04_310-0.84-0.86-0.71-0.73.h5</t>
-  </si>
-  <si>
-    <t>MFCC (max-min)</t>
-    <phoneticPr fontId="2"/>
-  </si>
-  <si>
-    <t>MFCC (z-score)</t>
-    <phoneticPr fontId="2"/>
+    <phoneticPr fontId="3"/>
+  </si>
+  <si>
+    <t>Best model name</t>
+    <phoneticPr fontId="3"/>
+  </si>
+  <si>
+    <t>MLP, Dataset 日本人 &amp; 外人増加 &amp; Augumentなし, epoch=500, Data数=37148</t>
+    <rPh sb="13" eb="16">
+      <t>ニホンジン</t>
+    </rPh>
+    <rPh sb="19" eb="21">
+      <t>ガイジン</t>
+    </rPh>
+    <rPh sb="21" eb="23">
+      <t>ゾウカ</t>
+    </rPh>
+    <rPh sb="53" eb="54">
+      <t>スウ</t>
+    </rPh>
+    <phoneticPr fontId="3"/>
+  </si>
+  <si>
+    <t>process_model_05_303-0.62-0.53-0.79-0.82.h5</t>
+  </si>
+  <si>
+    <t>process_model_06_310-0.84-0.86-0.71-0.73.h5</t>
+    <phoneticPr fontId="3"/>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="20" x14ac:knownFonts="1">
+  <fonts count="21" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
       <name val="游ゴシック"/>
       <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="游ゴシック"/>
+      <family val="2"/>
+      <charset val="128"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -818,134 +838,134 @@
   </borders>
   <cellStyleXfs count="43">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="9" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="10" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="11" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="5" borderId="12" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="6" borderId="13" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="6" borderId="12" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="14" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="7" borderId="15" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="9" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="10" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="11" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="5" borderId="12" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="6" borderId="13" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="6" borderId="12" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="14" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="7" borderId="15" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="17" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="8" borderId="16" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="17" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="8" borderId="16" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="15">
+  <cellXfs count="16">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
@@ -959,10 +979,13 @@
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="41" applyBorder="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="41" applyBorder="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="7" xfId="41" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="8" xfId="41" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="8" xfId="41" applyFont="1" applyBorder="1">
       <alignment vertical="center"/>
     </xf>
   </cellXfs>
@@ -1011,7 +1034,27 @@
     <cellStyle name="標準 2" xfId="41"/>
     <cellStyle name="良い" xfId="6" builtinId="26" customBuiltin="1"/>
   </cellStyles>
-  <dxfs count="15">
+  <dxfs count="17">
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C6500"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFEB9C"/>
+        </patternFill>
+      </fill>
+    </dxf>
     <dxf>
       <font>
         <color rgb="FF9C0006"/>
@@ -1440,13 +1483,13 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H51"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A28" workbookViewId="0">
-      <selection activeCell="B40" sqref="B40"/>
+    <sheetView tabSelected="1" topLeftCell="A31" workbookViewId="0">
+      <selection activeCell="A43" sqref="A43"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="18.75" x14ac:dyDescent="0.4"/>
   <cols>
-    <col min="1" max="1" width="42.25" customWidth="1"/>
+    <col min="1" max="1" width="34.25" customWidth="1"/>
     <col min="2" max="2" width="8.5" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="8.75" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="8.5" bestFit="1" customWidth="1"/>
@@ -1470,7 +1513,7 @@
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.4">
       <c r="A3" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="G3" s="10"/>
     </row>
@@ -1497,7 +1540,7 @@
         <v>8</v>
       </c>
       <c r="H4" s="3" t="s">
-        <v>16</v>
+        <v>44</v>
       </c>
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.4">
@@ -1549,7 +1592,7 @@
         <v>2.0309492308160499</v>
       </c>
       <c r="H6" s="6" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.4">
@@ -1575,7 +1618,7 @@
         <v>9.5017340121061906</v>
       </c>
       <c r="H7" s="6" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.4">
@@ -1601,7 +1644,7 @@
         <v>2.0301099735757502</v>
       </c>
       <c r="H8" s="6" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
     </row>
     <row r="9" spans="1:8" x14ac:dyDescent="0.4">
@@ -1631,7 +1674,7 @@
         <v>4.0645744385926603</v>
       </c>
       <c r="H10" s="6" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
     </row>
     <row r="11" spans="1:8" x14ac:dyDescent="0.4">
@@ -1657,7 +1700,7 @@
         <v>4.4434912619383402</v>
       </c>
       <c r="H11" s="6" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
     </row>
     <row r="12" spans="1:8" x14ac:dyDescent="0.4">
@@ -1683,7 +1726,7 @@
         <v>3.02813235987787</v>
       </c>
       <c r="H12" s="6" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
     </row>
     <row r="13" spans="1:8" x14ac:dyDescent="0.4">
@@ -1698,7 +1741,7 @@
     </row>
     <row r="14" spans="1:8" x14ac:dyDescent="0.4">
       <c r="A14" s="4" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="B14" s="11">
         <v>89.157300000000006</v>
@@ -1719,12 +1762,12 @@
         <v>3.3214287363964501</v>
       </c>
       <c r="H14" s="6" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
     </row>
     <row r="15" spans="1:8" x14ac:dyDescent="0.4">
       <c r="A15" s="4" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="B15" s="11">
         <v>89.388800000000003</v>
@@ -1745,7 +1788,7 @@
         <v>4.5268784792526899</v>
       </c>
       <c r="H15" s="6" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
     </row>
     <row r="16" spans="1:8" x14ac:dyDescent="0.4">
@@ -1760,7 +1803,7 @@
     </row>
     <row r="17" spans="1:8" x14ac:dyDescent="0.4">
       <c r="A17" s="7" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="B17" s="8">
         <v>90.227400000000003</v>
@@ -1781,12 +1824,12 @@
         <v>4.6358332903488799</v>
       </c>
       <c r="H17" s="9" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
     </row>
     <row r="20" spans="1:8" x14ac:dyDescent="0.4">
       <c r="A20" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="G20" s="10"/>
     </row>
@@ -1813,7 +1856,7 @@
         <v>8</v>
       </c>
       <c r="H21" s="3" t="s">
-        <v>16</v>
+        <v>44</v>
       </c>
     </row>
     <row r="22" spans="1:8" x14ac:dyDescent="0.4">
@@ -1839,7 +1882,7 @@
         <v>3.9272777458883699</v>
       </c>
       <c r="H22" s="6" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
     </row>
     <row r="23" spans="1:8" x14ac:dyDescent="0.4">
@@ -1865,7 +1908,7 @@
         <v>4.9420265101641396</v>
       </c>
       <c r="H23" s="6" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
     </row>
     <row r="24" spans="1:8" x14ac:dyDescent="0.4">
@@ -1891,7 +1934,7 @@
         <v>3.5370035549004801</v>
       </c>
       <c r="H24" s="6" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
     </row>
     <row r="25" spans="1:8" x14ac:dyDescent="0.4">
@@ -1917,7 +1960,7 @@
         <v>1.09861990451812</v>
       </c>
       <c r="H25" s="6" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
     </row>
     <row r="26" spans="1:8" x14ac:dyDescent="0.4">
@@ -1947,7 +1990,7 @@
         <v>3.5642465432409201</v>
       </c>
       <c r="H27" s="6" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
     </row>
     <row r="28" spans="1:8" x14ac:dyDescent="0.4">
@@ -1973,7 +2016,7 @@
         <v>4.0934476775152104</v>
       </c>
       <c r="H28" s="6" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
     </row>
     <row r="29" spans="1:8" x14ac:dyDescent="0.4">
@@ -1999,7 +2042,7 @@
         <v>3.4321631635513001</v>
       </c>
       <c r="H29" s="6" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
     </row>
     <row r="30" spans="1:8" x14ac:dyDescent="0.4">
@@ -2014,7 +2057,7 @@
     </row>
     <row r="31" spans="1:8" x14ac:dyDescent="0.4">
       <c r="A31" s="4" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="B31" s="11">
         <v>99.803899999999999</v>
@@ -2035,12 +2078,12 @@
         <v>4.6677117919918301</v>
       </c>
       <c r="H31" s="6" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
     </row>
     <row r="32" spans="1:8" x14ac:dyDescent="0.4">
       <c r="A32" s="4" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="B32" s="11">
         <v>99.866500000000002</v>
@@ -2061,7 +2104,7 @@
         <v>3.4994441684079298</v>
       </c>
       <c r="H32" s="6" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
     </row>
     <row r="33" spans="1:8" x14ac:dyDescent="0.4">
@@ -2076,7 +2119,7 @@
     </row>
     <row r="34" spans="1:8" x14ac:dyDescent="0.4">
       <c r="A34" s="7" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="B34" s="8">
         <v>72.454348206519995</v>
@@ -2097,12 +2140,12 @@
         <v>0.89249807596206598</v>
       </c>
       <c r="H34" s="9" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
     </row>
     <row r="37" spans="1:8" x14ac:dyDescent="0.4">
       <c r="A37" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
     </row>
     <row r="38" spans="1:8" x14ac:dyDescent="0.4">
@@ -2128,78 +2171,108 @@
         <v>8</v>
       </c>
       <c r="H38" s="3" t="s">
-        <v>16</v>
+        <v>44</v>
       </c>
     </row>
     <row r="39" spans="1:8" x14ac:dyDescent="0.4">
-      <c r="A39" s="4" t="s">
+      <c r="A39" s="7" t="s">
         <v>14</v>
       </c>
-      <c r="B39" s="11">
+      <c r="B39" s="12">
         <v>0.71</v>
       </c>
-      <c r="C39" s="11">
+      <c r="C39" s="12">
         <v>0.84</v>
       </c>
-      <c r="D39" s="11">
+      <c r="D39" s="12">
         <v>0.74</v>
       </c>
-      <c r="E39" s="11">
+      <c r="E39" s="12">
         <v>0.8</v>
       </c>
-      <c r="F39" s="14">
+      <c r="F39" s="13">
         <v>0.66355139017105103</v>
       </c>
-      <c r="G39" s="14">
+      <c r="G39" s="13">
         <v>1.05123579502105</v>
       </c>
-      <c r="H39" s="13" t="s">
-        <v>45</v>
+      <c r="H39" s="15" t="s">
+        <v>47</v>
       </c>
     </row>
     <row r="40" spans="1:8" x14ac:dyDescent="0.4">
-      <c r="A40" s="4" t="s">
-        <v>46</v>
-      </c>
+      <c r="A40" s="5"/>
       <c r="B40" s="11"/>
       <c r="C40" s="11"/>
       <c r="D40" s="5"/>
       <c r="E40" s="11"/>
       <c r="F40" s="5"/>
       <c r="G40" s="5"/>
-      <c r="H40" s="6"/>
+      <c r="H40" s="5"/>
     </row>
     <row r="41" spans="1:8" x14ac:dyDescent="0.4">
-      <c r="A41" s="7" t="s">
-        <v>47</v>
-      </c>
-      <c r="B41" s="12"/>
-      <c r="C41" s="12"/>
-      <c r="D41" s="8"/>
-      <c r="E41" s="12"/>
-      <c r="F41" s="8"/>
-      <c r="G41" s="8"/>
-      <c r="H41" s="9"/>
+      <c r="A41" s="11" t="s">
+        <v>45</v>
+      </c>
+      <c r="B41" s="11"/>
+      <c r="C41" s="11"/>
+      <c r="D41" s="5"/>
+      <c r="E41" s="11"/>
+      <c r="F41" s="5"/>
+      <c r="G41" s="5"/>
+      <c r="H41" s="5"/>
     </row>
     <row r="42" spans="1:8" x14ac:dyDescent="0.4">
-      <c r="A42" s="5"/>
-      <c r="B42" s="11"/>
-      <c r="C42" s="11"/>
-      <c r="D42" s="11"/>
-      <c r="E42" s="11"/>
-      <c r="F42" s="5"/>
-      <c r="G42" s="5"/>
-      <c r="H42" s="5"/>
+      <c r="A42" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="B42" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="C42" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="D42" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="E42" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="F42" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="G42" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="H42" s="3" t="s">
+        <v>44</v>
+      </c>
     </row>
     <row r="43" spans="1:8" x14ac:dyDescent="0.4">
-      <c r="A43" s="11"/>
-      <c r="B43" s="5"/>
-      <c r="C43" s="5"/>
-      <c r="D43" s="5"/>
-      <c r="E43" s="5"/>
-      <c r="F43" s="5"/>
-      <c r="G43" s="5"/>
-      <c r="H43" s="5"/>
+      <c r="A43" s="7" t="s">
+        <v>39</v>
+      </c>
+      <c r="B43" s="12">
+        <v>0.79</v>
+      </c>
+      <c r="C43" s="12">
+        <v>0.61</v>
+      </c>
+      <c r="D43" s="12">
+        <v>0.82</v>
+      </c>
+      <c r="E43" s="12">
+        <v>0.54</v>
+      </c>
+      <c r="F43" s="13">
+        <v>0.75848144292831399</v>
+      </c>
+      <c r="G43" s="13">
+        <v>0.74760383367538397</v>
+      </c>
+      <c r="H43" s="14" t="s">
+        <v>46</v>
+      </c>
     </row>
     <row r="44" spans="1:8" x14ac:dyDescent="0.4">
       <c r="A44" s="5"/>
@@ -2282,50 +2355,56 @@
       <c r="H51" s="5"/>
     </row>
   </sheetData>
-  <phoneticPr fontId="2"/>
+  <phoneticPr fontId="3"/>
   <conditionalFormatting sqref="F5:F8">
+    <cfRule type="top10" dxfId="16" priority="17" rank="1"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="F10:F12">
+    <cfRule type="top10" dxfId="15" priority="16" rank="1"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="F14:F15">
     <cfRule type="top10" dxfId="14" priority="15" rank="1"/>
   </conditionalFormatting>
-  <conditionalFormatting sqref="F10:F12">
+  <conditionalFormatting sqref="F17">
     <cfRule type="top10" dxfId="13" priority="14" rank="1"/>
   </conditionalFormatting>
-  <conditionalFormatting sqref="F14:F15">
+  <conditionalFormatting sqref="F22:F25">
     <cfRule type="top10" dxfId="12" priority="13" rank="1"/>
   </conditionalFormatting>
-  <conditionalFormatting sqref="F17">
+  <conditionalFormatting sqref="F27:F29">
     <cfRule type="top10" dxfId="11" priority="12" rank="1"/>
   </conditionalFormatting>
-  <conditionalFormatting sqref="F22:F25">
+  <conditionalFormatting sqref="F31:F32">
     <cfRule type="top10" dxfId="10" priority="11" rank="1"/>
   </conditionalFormatting>
-  <conditionalFormatting sqref="F27:F29">
+  <conditionalFormatting sqref="F34">
     <cfRule type="top10" dxfId="9" priority="10" rank="1"/>
   </conditionalFormatting>
-  <conditionalFormatting sqref="F31:F32">
+  <conditionalFormatting sqref="F5:F17">
     <cfRule type="top10" dxfId="8" priority="9" rank="1"/>
   </conditionalFormatting>
-  <conditionalFormatting sqref="F34">
+  <conditionalFormatting sqref="F22:F34">
     <cfRule type="top10" dxfId="7" priority="8" rank="1"/>
   </conditionalFormatting>
-  <conditionalFormatting sqref="F5:F17">
+  <conditionalFormatting sqref="F39:F41">
     <cfRule type="top10" dxfId="6" priority="7" rank="1"/>
   </conditionalFormatting>
-  <conditionalFormatting sqref="F22:F34">
+  <conditionalFormatting sqref="F44:F46">
     <cfRule type="top10" dxfId="5" priority="6" rank="1"/>
   </conditionalFormatting>
-  <conditionalFormatting sqref="F39:F42">
+  <conditionalFormatting sqref="F48:F49">
     <cfRule type="top10" dxfId="4" priority="5" rank="1"/>
   </conditionalFormatting>
-  <conditionalFormatting sqref="F44:F46">
+  <conditionalFormatting sqref="F51">
     <cfRule type="top10" dxfId="3" priority="4" rank="1"/>
   </conditionalFormatting>
-  <conditionalFormatting sqref="F48:F49">
+  <conditionalFormatting sqref="F39:F41 F44:F51">
     <cfRule type="top10" dxfId="2" priority="3" rank="1"/>
   </conditionalFormatting>
-  <conditionalFormatting sqref="F51">
+  <conditionalFormatting sqref="F43">
     <cfRule type="top10" dxfId="1" priority="2" rank="1"/>
   </conditionalFormatting>
-  <conditionalFormatting sqref="F39:F51">
+  <conditionalFormatting sqref="F43">
     <cfRule type="top10" dxfId="0" priority="1" rank="1"/>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>